<commit_message>
tomcat docker image 生成まで
</commit_message>
<xml_diff>
--- a/ecs-study/CodePipeline.xlsx
+++ b/ecs-study/CodePipeline.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
   <si>
     <t>※ CodePipeline で使う場合はバージョニングをする必要がある。(変更したら Pipeline が走る仕組みは、このバージョンを利用していると思う)</t>
     <rPh sb="16" eb="17">
@@ -693,15 +693,52 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>※ ここで CodePipeline 経由で Server Build ～ 試験 Docker Image ECR Push までが可能</t>
+    <t>※ ここで CodePipeline 経由で Server Build ～ Tomcat Docker Image ECR Push までが可能</t>
     <rPh sb="19" eb="21">
       <t>ケイユ</t>
     </rPh>
-    <rPh sb="38" eb="40">
-      <t>シケン</t>
-    </rPh>
-    <rPh sb="66" eb="68">
+    <rPh sb="70" eb="72">
       <t>カノウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>※ EC2 インスタンス上で、ECR より docker pull し、container 上で以下コールできる。</t>
+    <rPh sb="12" eb="13">
+      <t>ジョウ</t>
+    </rPh>
+    <rPh sb="46" eb="47">
+      <t>ジョウ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>イカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&gt; http://localhost:8080/ecs-system/app/ecs-server</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>War ファイルなどでも、さらに zip 化しないといけない点に注意</t>
+    <rPh sb="21" eb="22">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>テン</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>チュウイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>※ しなければ、war が解凍されたものが Source として送られる。</t>
+    <rPh sb="13" eb="15">
+      <t>カイトウ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>オク</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -2494,6 +2531,100 @@
         <a:effectLst/>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2049" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="200025" y="8791575"/>
+          <a:ext cx="6153150" cy="3543300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>552451</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="直線矢印コネクタ 16"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="5553076" y="12030075"/>
+          <a:ext cx="3457574" cy="409575"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3259,7 +3390,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:B16"/>
+  <dimension ref="B2:B19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3327,6 +3458,16 @@
     <row r="16" spans="2:2">
       <c r="B16" s="1" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -3637,6 +3778,16 @@
         <v>52</v>
       </c>
     </row>
+    <row r="83" spans="15:15">
+      <c r="O83" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="84" spans="15:15">
+      <c r="O84" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
     <row r="113" spans="15:15">
       <c r="O113" s="2" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
UI Component + formik
</commit_message>
<xml_diff>
--- a/ecs-study/CodePipeline.xlsx
+++ b/ecs-study/CodePipeline.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="23715" windowHeight="10305"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="23715" windowHeight="10305" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="目次" sheetId="6" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
   <si>
     <t>※ CodePipeline で使う場合はバージョニングをする必要がある。(変更したら Pipeline が走る仕組みは、このバージョンを利用していると思う)</t>
     <rPh sb="16" eb="17">
@@ -851,10 +851,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">   &gt; docker run -itd --net=host &lt;イメージID&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">   例: http://ec2-13-113-237-49.ap-northeast-1.compute.amazonaws.com:801/app/ecs-server</t>
     <rPh sb="3" eb="4">
       <t>レイ</t>
@@ -863,6 +859,18 @@
   </si>
   <si>
     <t xml:space="preserve">   &gt; http://&lt;ec2 public dns&gt;:801/app/ecs-server</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&gt; http://localhost:801/view/index.html</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   &gt; http://&lt;ec2 public dns&gt;:801/view/index.html</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   &gt; docker run -itd --net=host &lt;イメージID&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3513,9 +3521,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:B23"/>
+  <dimension ref="B2:B24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
@@ -3593,13 +3601,18 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="2:2">
-      <c r="B21" s="1" t="s">
+    <row r="20" spans="2:2">
+      <c r="B20" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="2:2">
-      <c r="B23" s="1" t="s">
+    <row r="24" spans="2:2">
+      <c r="B24" s="1" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4033,9 +4046,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:B21"/>
+  <dimension ref="B2:B23"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
@@ -4065,7 +4080,7 @@
     </row>
     <row r="7" spans="2:2">
       <c r="B7" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="2:2">
@@ -4100,21 +4115,31 @@
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="2:2">
-      <c r="B21" s="1" t="s">
+    <row r="23" spans="2:2">
+      <c r="B23" s="1" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>